<commit_message>
#Atualizaçao ConsultaCliente, ConsultaColetaCNT, FrmEditarColeta
</commit_message>
<xml_diff>
--- a/NewCapit/Uploads/ImportacaoCNT.xlsx
+++ b/NewCapit/Uploads/ImportacaoCNT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mauricio\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704D33DE-9554-4A7B-956F-B4FBFCA81D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22A7F4A-CCD3-4006-9EF3-E91D6F3EB921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DEDE3E4D-A464-4D49-ACAB-32D2A6C291CF}"/>
   </bookViews>
@@ -6527,8 +6527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2529AAF4-7417-4149-ABF3-2B41068F365E}">
   <dimension ref="A1:P1170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T18" sqref="T18"/>
+    <sheetView tabSelected="1" topLeftCell="A713" workbookViewId="0">
+      <selection activeCell="G724" sqref="G724"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>